<commit_message>
Fix project gantt chart
</commit_message>
<xml_diff>
--- a/ExampleFiles/projects.xlsx
+++ b/ExampleFiles/projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE04D3C-6283-4093-921B-F8B1562384BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BBCA36-4970-4836-AAFE-B3525DFBE64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>Dependencies</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>EstimatedEffortHours</t>
   </si>
   <si>
     <t>ProjectName</t>
@@ -101,14 +95,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}" name="Table1" displayName="Table1" ref="A1:E3" totalsRowShown="0">
-  <autoFilter ref="A1:E3" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C11070B8-C7FE-4695-859A-8CFBC6660079}" name="ID"/>
     <tableColumn id="2" xr3:uid="{86B04E0E-DD87-4469-B60B-B628A639FB53}" name="ProjectName"/>
-    <tableColumn id="4" xr3:uid="{1A614939-83A3-45A7-A1F6-C42770FF16D5}" name="EstimatedEffortHours"/>
     <tableColumn id="5" xr3:uid="{9730AFE1-7050-4486-AAC2-D57F321CD0FE}" name="Dependencies"/>
-    <tableColumn id="6" xr3:uid="{4F1650EA-3E7F-4399-AF87-7E47471B2DD0}" name="Progress"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -377,63 +369,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>170</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>125</v>
-      </c>
-      <c r="D3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add project and end week
</commit_message>
<xml_diff>
--- a/ExampleFiles/projects.xlsx
+++ b/ExampleFiles/projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BBCA36-4970-4836-AAFE-B3525DFBE64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FD87B2-D37F-4766-A730-7651FD10CD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="6840" windowWidth="11712" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Dependencies</t>
-  </si>
-  <si>
     <t>ProjectName</t>
   </si>
   <si>
@@ -40,6 +34,12 @@
   </si>
   <si>
     <t>Project B</t>
+  </si>
+  <si>
+    <t>ProjectID</t>
+  </si>
+  <si>
+    <t>ProjectDependency</t>
   </si>
 </sst>
 </file>
@@ -98,9 +98,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0">
   <autoFilter ref="A1:C3" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C11070B8-C7FE-4695-859A-8CFBC6660079}" name="ID"/>
+    <tableColumn id="1" xr3:uid="{C11070B8-C7FE-4695-859A-8CFBC6660079}" name="ProjectID"/>
     <tableColumn id="2" xr3:uid="{86B04E0E-DD87-4469-B60B-B628A639FB53}" name="ProjectName"/>
-    <tableColumn id="5" xr3:uid="{9730AFE1-7050-4486-AAC2-D57F321CD0FE}" name="Dependencies"/>
+    <tableColumn id="5" xr3:uid="{9730AFE1-7050-4486-AAC2-D57F321CD0FE}" name="ProjectDependency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,13 +384,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -398,7 +398,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -406,7 +406,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>

</xml_diff>

<commit_message>
Update excel files and default rules, and holidays
</commit_message>
<xml_diff>
--- a/ExampleFiles/projects.xlsx
+++ b/ExampleFiles/projects.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902CA519-824E-4364-912B-E558999282F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A6FB69-71A6-44A5-A5A2-D9318F2B5933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ProjectName</t>
   </si>
@@ -47,6 +46,9 @@
   </si>
   <si>
     <t>Project D</t>
+  </si>
+  <si>
+    <t>ProjectGroup</t>
   </si>
 </sst>
 </file>
@@ -102,12 +104,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}" name="Table1" displayName="Table1" ref="A1:D5" totalsRowShown="0">
+  <autoFilter ref="A1:D5" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C11070B8-C7FE-4695-859A-8CFBC6660079}" name="ProjectID"/>
     <tableColumn id="2" xr3:uid="{86B04E0E-DD87-4469-B60B-B628A639FB53}" name="ProjectName"/>
     <tableColumn id="5" xr3:uid="{9730AFE1-7050-4486-AAC2-D57F321CD0FE}" name="ProjectDependency"/>
+    <tableColumn id="3" xr3:uid="{C724CC67-BC67-4D14-B0D0-A8DAD866049F}" name="ProjectGroup"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -376,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -389,7 +392,7 @@
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -399,40 +402,52 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excel models and documentation
</commit_message>
<xml_diff>
--- a/ExampleFiles/projects.xlsx
+++ b/ExampleFiles/projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A6FB69-71A6-44A5-A5A2-D9318F2B5933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E08AE00-1E0E-47EF-BE17-1FF865D759CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="7845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,8 +424,11 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -436,7 +439,7 @@
         <v>5</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -447,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mock data and unit tests
</commit_message>
<xml_diff>
--- a/ExampleFiles/projects.xlsx
+++ b/ExampleFiles/projects.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353A4400-1028-482A-83AA-EEE5E1C18C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A02283E-F8E9-4518-B123-B2241749A773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="6840" windowWidth="11712" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>